<commit_message>
small changes to pipeline, working well
</commit_message>
<xml_diff>
--- a/Finances.xlsx
+++ b/Finances.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,6 +27,13 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,17 +59,20 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,11 +519,6 @@
           <t>Image</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Open File</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -529,27 +534,16 @@
       <c r="C2" t="n">
         <v>155000</v>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>MR JOHN HARRIS HOECKER ua: u.a. wow</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
+      <c r="O2" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1736234689919.jpeg</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -565,27 +559,16 @@
       <c r="C3" t="n">
         <v>1175</v>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
           <t>MR UTHALKAEWSR</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
+      <c r="O3" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1736263885083.jpeg</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -601,27 +584,16 @@
       <c r="C4" t="n">
         <v>520</v>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
           <t>MISSDAENG ARYEE</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
+      <c r="O4" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1736444388546.jpeg</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -637,27 +609,16 @@
       <c r="C5" t="n">
         <v>1920</v>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>MISSDAENG ARYEE</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr">
+      <c r="O5" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1736605759739.jpeg</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -673,27 +634,16 @@
       <c r="C6" t="n">
         <v>525</v>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>DRUG-MOBILE EXPO)</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr">
+      <c r="O6" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1736735599740.jpeg</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -709,27 +659,16 @@
       <c r="C7" t="n">
         <v>1280</v>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>MISSDAENG ARYEE</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr">
+      <c r="O7" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1736862361432.jpeg</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -745,27 +684,16 @@
       <c r="C8" t="n">
         <v>1850</v>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>usun lsowsnunansvinw t3gv?KU ina</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr">
+      <c r="O8" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1737711357865.jpeg</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -781,27 +709,16 @@
       <c r="C9" t="n">
         <v>1857</v>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
           <t>MS. WACHIRAPORN LE EPATANAKITJAROEN</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr">
+      <c r="O9" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1737980346979.jpeg</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -817,27 +734,16 @@
       <c r="C10" t="n">
         <v>75</v>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
           <t>MR. SITIDET LEEPATT HANAKITCHAREON</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr">
+      <c r="O10" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1738029890495.jpeg</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -853,27 +759,16 @@
       <c r="C11" t="n">
         <v>759</v>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
           <t>KANOKLAK NGA</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr">
+      <c r="O11" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1740307839454.jpeg</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -889,27 +784,16 @@
       <c r="C12" t="n">
         <v>871.2</v>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
           <t>BOUTIQUE HOUSE)</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr">
+      <c r="O12" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1740312104849.jpeg</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -925,27 +809,16 @@
       <c r="C13" t="n">
         <v>275</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t>MS. JENNIPHA PHONMAT</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr">
+      <c r="O13" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1741685313467.jpeg</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -961,27 +834,16 @@
       <c r="C14" t="n">
         <v>125</v>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
           <t>MS. YUWADEE KHAMAKSORN</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr">
+      <c r="O14" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1741686251347.jpeg</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -997,27 +859,16 @@
       <c r="C15" t="n">
         <v>1260</v>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
           <t>MISSDAENG ARYEE</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr">
+      <c r="O15" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1742218179862.jpeg</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1033,27 +884,16 @@
       <c r="C16" t="n">
         <v>300</v>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
           <t>MR.MONGKHON CHINARAT</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
+      <c r="O16" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1742296591508.jpeg</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1069,27 +909,16 @@
       <c r="C17" t="n">
         <v>909</v>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
           <t>CENTRAL BOUTIQUE HOUSE</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr">
+      <c r="O17" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1743249311896.jpeg</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1105,27 +934,16 @@
       <c r="C18" t="n">
         <v>275</v>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
           <t>MR. KORAKOTE RATTANASATEAN</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr">
+      <c r="O18" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1743414014339.jpeg</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1141,27 +959,16 @@
       <c r="C19" t="n">
         <v>600</v>
       </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
           <t>MR. THANAKRIT TOWICHAN</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr">
+      <c r="O19" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1743933397908.jpeg</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1177,27 +984,16 @@
       <c r="C20" t="n">
         <v>730</v>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
           <t>MS. PANICHA PHATTH ANATHAWONCHOT</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr">
+      <c r="O20" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1744039030770.jpeg</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1213,27 +1009,16 @@
       <c r="C21" t="n">
         <v>1850</v>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
           <t>usun lsowgnunansoinw t38v?KU na</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr">
+      <c r="O21" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1744966059264.jpeg</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1249,27 +1034,16 @@
       <c r="C22" t="n">
         <v>926.1</v>
       </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
           <t>CENTRAL BOUTIQUE HOUSE</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr">
+      <c r="O22" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1745323501043.jpeg</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1285,27 +1059,16 @@
       <c r="C23" t="n">
         <v>1223.1</v>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
           <t>CENTRAL BOUTIQUE HOUSE</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr">
+      <c r="O23" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1745756198010.jpeg</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1321,27 +1084,16 @@
       <c r="C24" t="n">
         <v>2870</v>
       </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
           <t>MISSDAENG ARYEE P</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr">
+      <c r="O24" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1746023374268.jpeg</t>
         </is>
       </c>
-      <c r="P24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1357,27 +1109,16 @@
       <c r="C25" t="n">
         <v>75000</v>
       </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
           <t>MR JOHN HARRIS HOECKER ua: u.a. wow</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr">
+      <c r="O25" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1746265274154.jpeg</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1393,27 +1134,16 @@
       <c r="C26" t="n">
         <v>600</v>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
           <t>MR. THANAKRIT TOWICHAN</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr">
+      <c r="O26" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1746523475665.jpeg</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1429,27 +1159,16 @@
       <c r="C27" t="n">
         <v>1850</v>
       </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
           <t>usun lsowgnunansoinw t38v?KU na</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr">
+      <c r="O27" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1746777843174.jpeg</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1465,27 +1184,16 @@
       <c r="C28" t="n">
         <v>300</v>
       </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
           <t>MR NATTHAPHAT THATSANEEYAPHAPP</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr">
+      <c r="O28" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1747128230438.jpeg</t>
         </is>
       </c>
-      <c r="P28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1501,27 +1209,16 @@
       <c r="C29" t="n">
         <v>210</v>
       </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
           <t>MR JOHN HARRIS HOECKER ua: u.a. wow</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr">
+      <c r="O29" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1747474030450.jpeg</t>
         </is>
       </c>
-      <c r="P29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1537,27 +1234,16 @@
       <c r="C30" t="n">
         <v>300</v>
       </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
           <t>MR. PATIPAN POUNGKUM</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr">
+      <c r="O30" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1748546495221.jpeg</t>
         </is>
       </c>
-      <c r="P30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1573,27 +1259,16 @@
       <c r="C31" t="n">
         <v>600</v>
       </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
           <t>MR. THANAKRIT TOWICHAN</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr">
+      <c r="O31" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1748586586145.jpeg</t>
         </is>
       </c>
-      <c r="P31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1609,27 +1284,16 @@
       <c r="C32" t="n">
         <v>6220</v>
       </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
           <t>usun lsowgnunansoinw t38v?KU na</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr">
+      <c r="O32" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1748591753296.jpeg</t>
         </is>
       </c>
-      <c r="P32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1645,27 +1309,16 @@
       <c r="C33" t="n">
         <v>2390</v>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
           <t>usun 5sauuna ina on</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr">
+      <c r="O33" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1751007967806.jpeg</t>
         </is>
       </c>
-      <c r="P33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1681,27 +1334,16 @@
       <c r="C34" t="n">
         <v>600</v>
       </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
           <t>MR. THANAKRIT TOWICHAN</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr">
+      <c r="O34" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1752041259549.jpeg</t>
         </is>
       </c>
-      <c r="P34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1717,27 +1359,16 @@
       <c r="C35" t="n">
         <v>6000</v>
       </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
           <t>MR.DORON PELED</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr">
+      <c r="O35" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1752477502193.jpeg</t>
         </is>
       </c>
-      <c r="P35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1753,27 +1384,16 @@
       <c r="C36" t="n">
         <v>700</v>
       </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
           <t>10 usun lsowgnunansvinw</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr">
+      <c r="O36" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1753087420488.jpeg</t>
         </is>
       </c>
-      <c r="P36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1789,27 +1409,16 @@
       <c r="C37" t="n">
         <v>2695</v>
       </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
           <t>10 usun Isvwsnunansoinw</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr">
+      <c r="O37" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1753508973280.jpeg</t>
         </is>
       </c>
-      <c r="P37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1825,31 +1434,21 @@
       <c r="C38" t="n">
         <v>600</v>
       </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
           <t>MR NATTHAPHAT THATSANEEYAPHAPP</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr">
         <is>
           <t>Taxi meeting</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr"/>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr">
+      <c r="O38" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1756638501795.jpeg</t>
         </is>
       </c>
-      <c r="P38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1865,31 +1464,21 @@
       <c r="C39" t="n">
         <v>150000</v>
       </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
           <t>MR JOHN HARRIS HOECKER ua: u.a. wuw</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr">
         <is>
           <t>Household</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr"/>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr">
+      <c r="O39" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1756659795578.jpeg</t>
         </is>
       </c>
-      <c r="P39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1905,31 +1494,21 @@
       <c r="C40" t="n">
         <v>10000</v>
       </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
           <t>MR JOHN HARRIS HOECKER ua: u.a. wuw</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr">
         <is>
           <t>Household</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr"/>
-      <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr">
+      <c r="O40" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1756690238117.jpeg</t>
         </is>
       </c>
-      <c r="P40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1945,31 +1524,21 @@
       <c r="C41" t="n">
         <v>10000</v>
       </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
           <t>MR JOHN HARRIS HOECKER ua: u.a. wuw</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr">
         <is>
           <t>Household</t>
         </is>
       </c>
-      <c r="J41" t="inlineStr"/>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr">
+      <c r="O41" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1756712860983.jpeg</t>
         </is>
       </c>
-      <c r="P41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1985,31 +1554,21 @@
       <c r="C42" t="n">
         <v>1050.74</v>
       </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
           <t>AWNPostpaid Dav</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr">
         <is>
           <t>Phone</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr">
+      <c r="O42" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1757031087957.jpeg</t>
         </is>
       </c>
-      <c r="P42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2025,31 +1584,21 @@
       <c r="C43" t="n">
         <v>600</v>
       </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
           <t>MR NATTHAPHAT THATSANEEYAPHAPP</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr">
         <is>
           <t>Taxi meeting</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr"/>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr">
+      <c r="O43" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1757065067465.jpeg</t>
         </is>
       </c>
-      <c r="P43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2065,33 +1614,68 @@
       <c r="C44" t="n">
         <v>2500</v>
       </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
           <t>usun lsowsunansvinw</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr">
         <is>
           <t>physical therapy</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr"/>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr">
+      <c r="O44" s="2" t="inlineStr">
         <is>
           <t>BBl-Screenshot-1757139772833.jpeg</t>
         </is>
       </c>
-      <c r="P44" t="inlineStr"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O8" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O9" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O10" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O11" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O12" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O13" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O14" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O15" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O16" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O17" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O18" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O19" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O20" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O21" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O22" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O23" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O24" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O25" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O26" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O27" r:id="rId26"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O28" r:id="rId27"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O29" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O30" r:id="rId29"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O31" r:id="rId30"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O32" r:id="rId31"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O33" r:id="rId32"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O34" r:id="rId33"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O35" r:id="rId34"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O36" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O37" r:id="rId36"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O38" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O39" r:id="rId38"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O40" r:id="rId39"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O41" r:id="rId40"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O42" r:id="rId41"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O43" r:id="rId42"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O44" r:id="rId43"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>